<commit_message>
top 3 i dla dwoch velocity bins
</commit_message>
<xml_diff>
--- a/Przykladowy Folder/wyniki/wyniki_średnie.xlsx
+++ b/Przykladowy Folder/wyniki/wyniki_średnie.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,181 +448,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0-5</t>
+          <t>10-15</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.257502336025</v>
+        <v>4.133277868047619</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10-15</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>3.4966084535</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>15-20</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3.818733325153572</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>20-25</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>3.097823182417857</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>25-30</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>2.201666647682937</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>30-35</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>7.315225330314286</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>35-40</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>5.851708746771428</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>40-45</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>2.265109933314286</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>45-50</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.5968896003857143</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
           <t>5-10</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>3.162000320575</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>50-55</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.5716138252571429</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>55-60</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0.5497297599857143</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>60-65</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0.5314890346428571</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>65-70</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0.2894107939285714</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>70-75</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.06791093977551023</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>75-80</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0.1814106407857143</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>80-85</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0.2046908479</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>85-90</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.07929484766666667</v>
+      <c r="B3" t="n">
+        <v>3.903367674083333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>